<commit_message>
Commit day4 logic building
</commit_message>
<xml_diff>
--- a/Goals and Tasks.xlsx
+++ b/Goals and Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanja\Documents\GitHub\AI-Python_Deeplearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4875B7F5-9FD9-46A0-808A-0699EAF5AB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA8EDA6-50EB-4D46-9DE9-959A6C53B45D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" state="hidden" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="387">
   <si>
     <t>Phase</t>
   </si>
@@ -1185,6 +1185,9 @@
   </si>
   <si>
     <t>project-employees-i</t>
+  </si>
+  <si>
+    <t>Working with Your Own Data and Documents in Python 2</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1388,13 +1391,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1408,9 +1432,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1427,27 +1448,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4278,7 +4280,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="35" t="s">
         <v>320</v>
       </c>
       <c r="B1" t="s">
@@ -4286,37 +4288,37 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
+      <c r="A2" s="35"/>
       <c r="B2" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
+      <c r="A3" s="35"/>
       <c r="B3" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="35"/>
       <c r="B4" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="35"/>
       <c r="B5" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="A6" s="35"/>
       <c r="B6" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="35"/>
       <c r="B7" t="s">
         <v>324</v>
       </c>
@@ -4364,10 +4366,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
@@ -4378,8 +4380,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" t="s">
         <v>19</v>
       </c>
@@ -4388,8 +4390,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" t="s">
         <v>24</v>
       </c>
@@ -4410,8 +4412,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
       <c r="C5" t="s">
         <v>29</v>
       </c>
@@ -4426,8 +4428,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
       <c r="C6" t="s">
         <v>34</v>
       </c>
@@ -4436,8 +4438,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" t="s">
         <v>39</v>
       </c>
@@ -4446,8 +4448,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
       <c r="C8" t="s">
         <v>44</v>
       </c>
@@ -4456,8 +4458,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C9" t="s">
@@ -4468,8 +4470,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C10" t="s">
@@ -4480,8 +4482,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C11" t="s">
@@ -4492,8 +4494,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C12" t="s">
@@ -4504,8 +4506,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C13" t="s">
@@ -4516,8 +4518,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C14" t="s">
@@ -4528,8 +4530,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35" t="s">
         <v>49</v>
       </c>
       <c r="C15" t="s">
@@ -4540,8 +4542,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C16" t="s">
@@ -4552,8 +4554,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C17" t="s">
@@ -4564,8 +4566,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18" t="s">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C18" t="s">
@@ -4576,8 +4578,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C19" t="s">
@@ -4588,8 +4590,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C20" t="s">
@@ -4600,8 +4602,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C21" t="s">
@@ -4612,8 +4614,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="35" t="s">
         <v>78</v>
       </c>
       <c r="C22" t="s">
@@ -4624,8 +4626,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="35"/>
+      <c r="B23" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C23" t="s">
@@ -4636,8 +4638,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C24" t="s">
@@ -4648,8 +4650,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C25" t="s">
@@ -4660,8 +4662,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C26" t="s">
@@ -4672,8 +4674,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18" t="s">
+      <c r="A27" s="35"/>
+      <c r="B27" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C27" t="s">
@@ -4684,8 +4686,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C28" t="s">
@@ -4696,8 +4698,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18" t="s">
+      <c r="A29" s="35"/>
+      <c r="B29" s="35" t="s">
         <v>102</v>
       </c>
       <c r="C29" t="s">
@@ -4708,10 +4710,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C30" t="s">
@@ -4722,8 +4724,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18" t="s">
+      <c r="A31" s="35"/>
+      <c r="B31" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C31" t="s">
@@ -4734,8 +4736,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18" t="s">
+      <c r="A32" s="35"/>
+      <c r="B32" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C32" t="s">
@@ -4746,8 +4748,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18" t="s">
+      <c r="A33" s="35"/>
+      <c r="B33" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C33" t="s">
@@ -4758,8 +4760,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18" t="s">
+      <c r="A34" s="35"/>
+      <c r="B34" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C34" t="s">
@@ -4770,8 +4772,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18" t="s">
+      <c r="A35" s="35"/>
+      <c r="B35" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C35" t="s">
@@ -4782,8 +4784,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18" t="s">
+      <c r="A36" s="35"/>
+      <c r="B36" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C36" t="s">
@@ -4794,8 +4796,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18" t="s">
+      <c r="A37" s="35"/>
+      <c r="B37" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C37" t="s">
@@ -4806,8 +4808,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18" t="s">
+      <c r="A38" s="35"/>
+      <c r="B38" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C38" t="s">
@@ -4818,8 +4820,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18" t="s">
+      <c r="A39" s="35"/>
+      <c r="B39" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C39" t="s">
@@ -4830,8 +4832,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18" t="s">
+      <c r="A40" s="35"/>
+      <c r="B40" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C40" t="s">
@@ -4842,8 +4844,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18" t="s">
+      <c r="A41" s="35"/>
+      <c r="B41" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C41" t="s">
@@ -4854,8 +4856,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18" t="s">
+      <c r="A42" s="35"/>
+      <c r="B42" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C42" t="s">
@@ -4866,8 +4868,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18" t="s">
+      <c r="A43" s="35"/>
+      <c r="B43" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C43" t="s">
@@ -4878,8 +4880,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18" t="s">
+      <c r="A44" s="35"/>
+      <c r="B44" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C44" t="s">
@@ -4890,8 +4892,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18" t="s">
+      <c r="A45" s="35"/>
+      <c r="B45" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C45" t="s">
@@ -4902,8 +4904,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18" t="s">
+      <c r="A46" s="35"/>
+      <c r="B46" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C46" t="s">
@@ -4914,8 +4916,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18" t="s">
+      <c r="A47" s="35"/>
+      <c r="B47" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C47" t="s">
@@ -4926,8 +4928,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="18" t="s">
+      <c r="A48" s="35"/>
+      <c r="B48" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C48" t="s">
@@ -4938,8 +4940,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="18" t="s">
+      <c r="A49" s="35"/>
+      <c r="B49" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C49" t="s">
@@ -4950,8 +4952,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="18" t="s">
+      <c r="A50" s="35"/>
+      <c r="B50" s="35" t="s">
         <v>176</v>
       </c>
       <c r="C50" t="s">
@@ -4962,8 +4964,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="18"/>
-      <c r="B51" s="18" t="s">
+      <c r="A51" s="35"/>
+      <c r="B51" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C51" t="s">
@@ -4974,8 +4976,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="18" t="s">
+      <c r="A52" s="35"/>
+      <c r="B52" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C52" t="s">
@@ -4986,8 +4988,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18" t="s">
+      <c r="A53" s="35"/>
+      <c r="B53" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C53" t="s">
@@ -4998,8 +5000,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="18" t="s">
+      <c r="A54" s="35"/>
+      <c r="B54" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C54" t="s">
@@ -5010,8 +5012,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="18"/>
-      <c r="B55" s="18" t="s">
+      <c r="A55" s="35"/>
+      <c r="B55" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C55" t="s">
@@ -5022,8 +5024,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18" t="s">
+      <c r="A56" s="35"/>
+      <c r="B56" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C56" t="s">
@@ -5034,8 +5036,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18" t="s">
+      <c r="A57" s="35"/>
+      <c r="B57" s="35" t="s">
         <v>199</v>
       </c>
       <c r="C57" t="s">
@@ -5046,10 +5048,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C58" t="s">
@@ -5060,8 +5062,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="18" t="s">
+      <c r="A59" s="35"/>
+      <c r="B59" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C59" t="s">
@@ -5072,8 +5074,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18" t="s">
+      <c r="A60" s="35"/>
+      <c r="B60" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C60" t="s">
@@ -5084,8 +5086,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18" t="s">
+      <c r="A61" s="35"/>
+      <c r="B61" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C61" t="s">
@@ -5096,8 +5098,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18" t="s">
+      <c r="A62" s="35"/>
+      <c r="B62" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C62" t="s">
@@ -5108,8 +5110,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18" t="s">
+      <c r="A63" s="35"/>
+      <c r="B63" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C63" t="s">
@@ -5120,8 +5122,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
-      <c r="B64" s="18" t="s">
+      <c r="A64" s="35"/>
+      <c r="B64" s="35" t="s">
         <v>224</v>
       </c>
       <c r="C64" t="s">
@@ -5132,8 +5134,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18" t="s">
+      <c r="A65" s="35"/>
+      <c r="B65" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C65" t="s">
@@ -5144,8 +5146,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18" t="s">
+      <c r="A66" s="35"/>
+      <c r="B66" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C66" t="s">
@@ -5156,8 +5158,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="18" t="s">
+      <c r="A67" s="35"/>
+      <c r="B67" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C67" t="s">
@@ -5168,8 +5170,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18" t="s">
+      <c r="A68" s="35"/>
+      <c r="B68" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C68" t="s">
@@ -5180,8 +5182,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18" t="s">
+      <c r="A69" s="35"/>
+      <c r="B69" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C69" t="s">
@@ -5192,8 +5194,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="18" t="s">
+      <c r="A70" s="35"/>
+      <c r="B70" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C70" t="s">
@@ -5204,8 +5206,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18" t="s">
+      <c r="A71" s="35"/>
+      <c r="B71" s="35" t="s">
         <v>249</v>
       </c>
       <c r="C71" t="s">
@@ -5216,8 +5218,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="18" t="s">
+      <c r="A72" s="35"/>
+      <c r="B72" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C72" t="s">
@@ -5228,8 +5230,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="18"/>
-      <c r="B73" s="18" t="s">
+      <c r="A73" s="35"/>
+      <c r="B73" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C73" t="s">
@@ -5240,8 +5242,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="18"/>
-      <c r="B74" s="18" t="s">
+      <c r="A74" s="35"/>
+      <c r="B74" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C74" t="s">
@@ -5252,8 +5254,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="18"/>
-      <c r="B75" s="18" t="s">
+      <c r="A75" s="35"/>
+      <c r="B75" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C75" t="s">
@@ -5264,8 +5266,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="18"/>
-      <c r="B76" s="18" t="s">
+      <c r="A76" s="35"/>
+      <c r="B76" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C76" t="s">
@@ -5276,8 +5278,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="18"/>
-      <c r="B77" s="18" t="s">
+      <c r="A77" s="35"/>
+      <c r="B77" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C77" t="s">
@@ -5288,8 +5290,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="18"/>
-      <c r="B78" s="18" t="s">
+      <c r="A78" s="35"/>
+      <c r="B78" s="35" t="s">
         <v>273</v>
       </c>
       <c r="C78" t="s">
@@ -5300,8 +5302,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18" t="s">
+      <c r="A79" s="35"/>
+      <c r="B79" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C79" t="s">
@@ -5312,8 +5314,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="18" t="s">
+      <c r="A80" s="35"/>
+      <c r="B80" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C80" t="s">
@@ -5324,8 +5326,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="18"/>
-      <c r="B81" s="18" t="s">
+      <c r="A81" s="35"/>
+      <c r="B81" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C81" t="s">
@@ -5336,8 +5338,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18" t="s">
+      <c r="A82" s="35"/>
+      <c r="B82" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C82" t="s">
@@ -5348,8 +5350,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="18"/>
-      <c r="B83" s="18" t="s">
+      <c r="A83" s="35"/>
+      <c r="B83" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C83" t="s">
@@ -5360,8 +5362,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="18"/>
-      <c r="B84" s="18" t="s">
+      <c r="A84" s="35"/>
+      <c r="B84" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C84" t="s">
@@ -5372,8 +5374,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18" t="s">
+      <c r="A85" s="35"/>
+      <c r="B85" s="35" t="s">
         <v>296</v>
       </c>
       <c r="C85" t="s">
@@ -5543,8 +5545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE52335-7D91-466B-9120-E00FFD104A09}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5562,30 +5564,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34" t="s">
         <v>365</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="19" t="s">
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -5616,17 +5618,17 @@
         <v>367</v>
       </c>
       <c r="L2" s="8"/>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
     </row>
     <row r="3" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
       <c r="B3">
@@ -5635,52 +5637,52 @@
       <c r="C3" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="18">
         <v>46059</v>
       </c>
       <c r="E3" t="s">
         <v>355</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="18">
         <v>46059</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="18">
         <v>46060</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="25"/>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>352</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="18"/>
       <c r="E4" t="s">
         <v>355</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
     </row>
     <row r="5" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="10">
         <v>3</v>
       </c>
@@ -5696,19 +5698,19 @@
       <c r="F5" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="17"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+      <c r="A6" s="25">
         <v>2</v>
       </c>
       <c r="B6">
@@ -5717,79 +5719,79 @@
       <c r="C6" t="s">
         <v>359</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="18">
         <v>46060</v>
       </c>
       <c r="E6" t="s">
         <v>355</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="18">
         <v>46060</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
+      <c r="I6" s="18"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="25"/>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>362</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="18"/>
       <c r="E7" t="s">
         <v>355</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="25"/>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>363</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="18"/>
       <c r="E8" t="s">
         <v>355</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
     </row>
     <row r="9" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="10">
         <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="10" t="s">
         <v>355</v>
       </c>
@@ -5797,18 +5799,18 @@
       <c r="G9" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="17"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
+      <c r="A10" s="25">
         <v>3</v>
       </c>
       <c r="B10">
@@ -5826,12 +5828,12 @@
       <c r="F10" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="18">
         <v>46062</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="25"/>
       <c r="B11">
         <v>9</v>
       </c>
@@ -5850,10 +5852,10 @@
       <c r="H11" s="3">
         <v>46061</v>
       </c>
-      <c r="I11" s="17"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="25"/>
       <c r="B12">
         <v>10</v>
       </c>
@@ -5869,13 +5871,13 @@
       <c r="G12" t="s">
         <v>381</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="18">
         <v>46062</v>
       </c>
-      <c r="I12" s="17"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="10">
         <v>11</v>
       </c>
@@ -5894,69 +5896,70 @@
       <c r="G13" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="17"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="18"/>
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="30">
+      <c r="A14" s="16">
         <v>4</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="20" t="s">
         <v>385</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="22">
         <v>46062</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="F14" s="37"/>
+      <c r="F14" s="23"/>
       <c r="G14" t="s">
         <v>381</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="18">
         <v>46062</v>
       </c>
-      <c r="I14" s="17"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="10">
         <v>13</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="38"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="18"/>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
         <v>5</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="29" t="s">
+      <c r="G16" t="s">
         <v>383</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="22">
         <v>46063</v>
       </c>
-      <c r="L16" s="9"/>
+      <c r="I16" s="18">
+        <v>46064</v>
+      </c>
     </row>
     <row r="17" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="10">
         <v>15</v>
       </c>
@@ -5964,16 +5967,24 @@
       <c r="G17" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="H17" s="33">
-        <v>46063</v>
-      </c>
+      <c r="H17" s="19"/>
+      <c r="I17" s="35"/>
       <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="15">
+        <v>6</v>
+      </c>
       <c r="B18">
         <v>16</v>
       </c>
+      <c r="G18" s="10" t="s">
+        <v>386</v>
+      </c>
+      <c r="H18" s="3">
+        <v>46064</v>
+      </c>
+      <c r="I18" s="35"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
@@ -6031,7 +6042,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:F27" xr:uid="{CAE52335-7D91-466B-9120-E00FFD104A09}"/>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="M2:R9"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I10:I15"/>
@@ -6041,20 +6065,9 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="A10:A13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="I3:I9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="M2:R9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="D3:D4"/>
     <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>